<commit_message>
SPRINT 1: Initial setup test
</commit_message>
<xml_diff>
--- a/Documentation/Planning.xlsx
+++ b/Documentation/Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F935C2E2-7480-440F-9E1A-68AA5BF260C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6412019F-A4F1-49F9-B6DA-9FC35644EBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,168 +463,6 @@
     <xf numFmtId="16" fontId="1" fillId="7" borderId="1" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -652,24 +490,24 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -679,11 +517,173 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -977,7 +977,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,19 +996,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1032,20 +1032,20 @@
       <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38" t="s">
+      <c r="I2" s="85"/>
+      <c r="J2" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="38"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="11">
         <v>45199</v>
       </c>
@@ -1058,21 +1058,21 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="18" t="s">
+      <c r="I3" s="48"/>
+      <c r="J3" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="19"/>
+      <c r="K3" s="66"/>
     </row>
     <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="11">
         <v>45203</v>
       </c>
@@ -1085,19 +1085,19 @@
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="80" t="s">
+      <c r="G4" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="53"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="72"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
+    </row>
+    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="48"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="11">
         <v>45205</v>
       </c>
@@ -1110,19 +1110,19 @@
       <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="53"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="72"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="11">
         <v>45206</v>
       </c>
@@ -1135,19 +1135,19 @@
       <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="54" t="s">
+      <c r="G6" s="32"/>
+      <c r="H6" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="53"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="73"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="12"/>
       <c r="D7" s="3" t="s">
         <v>18</v>
@@ -1156,19 +1156,19 @@
         <v>2</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="68"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
         <v>19</v>
@@ -1177,17 +1177,17 @@
         <v>1</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="56" t="s">
+      <c r="G8" s="28"/>
+      <c r="H8" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
     </row>
     <row r="9" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
-      <c r="B9" s="73"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="12"/>
       <c r="D9" s="3" t="s">
         <v>20</v>
@@ -1196,32 +1196,32 @@
         <v>1</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="58" t="s">
+      <c r="G9" s="28"/>
+      <c r="H9" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="57"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="68"/>
     </row>
     <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="73"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="12"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="72"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="11">
         <v>45212</v>
       </c>
@@ -1231,22 +1231,22 @@
       <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F11" s="71">
+      <c r="F11" s="54">
         <v>6</v>
       </c>
-      <c r="G11" s="81" t="s">
+      <c r="G11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="11">
         <v>45219</v>
       </c>
@@ -1256,52 +1256,54 @@
       <c r="E12" s="2">
         <v>5</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="53" t="s">
+      <c r="F12" s="55"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="53"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="11">
+        <v>45212</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="53" t="s">
+      <c r="F13" s="55"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="53"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="72"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="11"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="70"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="13">
         <v>45207</v>
       </c>
@@ -1311,24 +1313,24 @@
       <c r="E15" s="7">
         <v>3</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="45">
         <v>4</v>
       </c>
-      <c r="G15" s="87" t="s">
+      <c r="G15" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="90" t="s">
+      <c r="H15" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="91"/>
-      <c r="J15" s="39" t="s">
+      <c r="I15" s="59"/>
+      <c r="J15" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="40"/>
+      <c r="K15" s="87"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="74"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="13">
         <v>45208</v>
       </c>
@@ -1338,52 +1340,54 @@
       <c r="E16" s="7">
         <v>3</v>
       </c>
-      <c r="F16" s="69"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="52" t="s">
+      <c r="F16" s="46"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="42"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="89"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="13">
+        <v>45207</v>
+      </c>
       <c r="D17" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="51" t="s">
+      <c r="F17" s="46"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="51"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="89"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="74"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="13"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="44"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="91"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="75"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="14">
         <v>45208</v>
       </c>
@@ -1393,24 +1397,24 @@
       <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="65">
+      <c r="F19" s="36">
         <v>5</v>
       </c>
-      <c r="G19" s="65" t="s">
+      <c r="G19" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="24" t="s">
+      <c r="I19" s="61"/>
+      <c r="J19" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="25"/>
+      <c r="K19" s="72"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="75"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="14">
         <v>45210</v>
       </c>
@@ -1420,118 +1424,120 @@
       <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="50" t="s">
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="50"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="74"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="14">
+        <v>45208</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="50" t="s">
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="50"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="74"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="75"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="14"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="74"/>
     </row>
     <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="76"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="15"/>
       <c r="D23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="49" t="s">
+      <c r="G23" s="39"/>
+      <c r="H23" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="49"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="74"/>
     </row>
     <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="76"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="15"/>
       <c r="D24" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="49" t="s">
+      <c r="G24" s="40"/>
+      <c r="H24" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="49"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="74"/>
     </row>
     <row r="25" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="76"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="15"/>
       <c r="D25" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="49" t="s">
+      <c r="G25" s="40"/>
+      <c r="H25" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="49"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="27"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="74"/>
     </row>
     <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="76"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="27"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="74"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="75"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="14">
         <v>45221</v>
       </c>
@@ -1541,22 +1547,22 @@
       <c r="E27" s="5">
         <v>3</v>
       </c>
-      <c r="F27" s="65">
+      <c r="F27" s="36">
         <v>8</v>
       </c>
-      <c r="G27" s="65" t="s">
+      <c r="G27" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="50" t="s">
+      <c r="H27" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="27"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="74"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="75"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="14">
         <v>45224</v>
       </c>
@@ -1566,118 +1572,120 @@
       <c r="E28" s="5">
         <v>3</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="50" t="s">
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="50"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="27"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="74"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="14"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="14">
+        <v>45221</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="5">
         <v>2</v>
       </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="50" t="s">
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="50"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="27"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="74"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="75"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="14"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="27"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="74"/>
     </row>
     <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="76"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="15"/>
       <c r="D31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="49" t="s">
+      <c r="G31" s="39"/>
+      <c r="H31" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="49"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="27"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="74"/>
     </row>
     <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="76"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="15"/>
       <c r="D32" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="49" t="s">
+      <c r="G32" s="40"/>
+      <c r="H32" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="49"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="27"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="74"/>
     </row>
     <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="76"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="15"/>
       <c r="D33" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="49" t="s">
+      <c r="G33" s="40"/>
+      <c r="H33" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="49"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="27"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="74"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="76"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="29"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="77"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="16">
         <v>45219</v>
       </c>
@@ -1687,24 +1695,24 @@
       <c r="E35" s="4">
         <v>2</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="42">
         <v>7</v>
       </c>
-      <c r="G35" s="59" t="s">
+      <c r="G35" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="47" t="s">
+      <c r="H35" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="47"/>
-      <c r="J35" s="30" t="s">
+      <c r="I35" s="64"/>
+      <c r="J35" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="K35" s="31"/>
+      <c r="K35" s="78"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="77"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="16">
         <v>45221</v>
       </c>
@@ -1714,52 +1722,54 @@
       <c r="E36" s="4">
         <v>2</v>
       </c>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="47" t="s">
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I36" s="47"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="33"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="80"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="16"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="16">
+        <v>45219</v>
+      </c>
       <c r="D37" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E37" s="4">
         <v>1</v>
       </c>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="47" t="s">
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="47"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="33"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="80"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="64"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="16"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="33"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="80"/>
     </row>
     <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="78"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="17"/>
       <c r="D39" s="10" t="s">
         <v>18</v>
@@ -1767,16 +1777,16 @@
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="48" t="s">
+      <c r="H39" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="33"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="80"/>
     </row>
     <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="78"/>
+      <c r="A40" s="63"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="17"/>
       <c r="D40" s="10" t="s">
         <v>19</v>
@@ -1784,16 +1794,16 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="48" t="s">
+      <c r="H40" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="48"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="33"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="79"/>
+      <c r="K40" s="80"/>
     </row>
     <row r="41" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
-      <c r="B41" s="78"/>
+      <c r="A41" s="63"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="17"/>
       <c r="D41" s="10" t="s">
         <v>20</v>
@@ -1801,31 +1811,31 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="H41" s="48" t="s">
+      <c r="H41" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="48"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="33"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="80"/>
     </row>
     <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="78"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="17"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="33"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="79"/>
+      <c r="K42" s="80"/>
     </row>
     <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="77"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="16"/>
       <c r="D43" s="4" t="s">
         <v>18</v>
@@ -1833,16 +1843,16 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="47" t="s">
+      <c r="H43" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="47"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="33"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="79"/>
+      <c r="K43" s="80"/>
     </row>
     <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
-      <c r="B44" s="77"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="16"/>
       <c r="D44" s="4" t="s">
         <v>19</v>
@@ -1850,16 +1860,16 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="47" t="s">
+      <c r="H44" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="47"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="33"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="80"/>
     </row>
     <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
-      <c r="B45" s="77"/>
+      <c r="A45" s="64"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="16"/>
       <c r="D45" s="4" t="s">
         <v>20</v>
@@ -1867,25 +1877,25 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="47" t="s">
+      <c r="H45" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I45" s="47"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="33"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="80"/>
     </row>
     <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
-      <c r="B46" s="77"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="16"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="35"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="81"/>
+      <c r="K46" s="82"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:K46" xr:uid="{784DA642-760B-4062-9544-643C79FF24CC}">
@@ -1893,69 +1903,6 @@
     <filterColumn colId="9" showButton="0"/>
   </autoFilter>
   <mergeCells count="76">
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
     <mergeCell ref="J3:K14"/>
     <mergeCell ref="J19:K34"/>
     <mergeCell ref="J35:K46"/>
@@ -1969,6 +1916,69 @@
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="A39:A42"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="G23:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding issues to the planning doc
</commit_message>
<xml_diff>
--- a/Documentation/Planning.xlsx
+++ b/Documentation/Planning.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6412019F-A4F1-49F9-B6DA-9FC35644EBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF7E693-23A3-5B4A-BEB3-45C1B8A186CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,21 +463,6 @@
     <xf numFmtId="16" fontId="1" fillId="7" borderId="1" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -490,6 +475,180 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -499,15 +658,9 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -516,174 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -977,40 +962,40 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="24.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-    </row>
-    <row r="2" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+    </row>
+    <row r="2" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1032,20 +1017,22 @@
       <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="85"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="K2" s="42"/>
+    </row>
+    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
       <c r="C3" s="11">
         <v>45199</v>
       </c>
@@ -1058,21 +1045,23 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="65" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="66"/>
-    </row>
-    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="18"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="57"/>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
       <c r="C4" s="11">
         <v>45203</v>
       </c>
@@ -1085,19 +1074,21 @@
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="48"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="68"/>
-    </row>
-    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="18"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="57"/>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
       <c r="C5" s="11">
         <v>45205</v>
       </c>
@@ -1110,19 +1101,21 @@
       <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="68"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="18"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="57"/>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
       <c r="C6" s="11">
         <v>45206</v>
       </c>
@@ -1135,19 +1128,19 @@
       <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="49" t="s">
+      <c r="G6" s="73"/>
+      <c r="H6" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="I6" s="57"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="12"/>
       <c r="D7" s="3" t="s">
         <v>18</v>
@@ -1156,19 +1149,19 @@
         <v>2</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="68"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="19"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
         <v>19</v>
@@ -1177,17 +1170,17 @@
         <v>1</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="51" t="s">
+      <c r="G8" s="81"/>
+      <c r="H8" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="68"/>
-    </row>
-    <row r="9" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="19"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="62"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="12"/>
       <c r="D9" s="3" t="s">
         <v>20</v>
@@ -1196,32 +1189,34 @@
         <v>1</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="53" t="s">
+      <c r="G9" s="81"/>
+      <c r="H9" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="52"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="68"/>
-    </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="19"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="62"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="12"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="G10" s="82"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
       <c r="C11" s="11">
         <v>45212</v>
       </c>
@@ -1231,22 +1226,24 @@
       <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="58">
         <v>6</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="48"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="68"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="18"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="57"/>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
       <c r="C12" s="11">
         <v>45219</v>
       </c>
@@ -1256,18 +1253,20 @@
       <c r="E12" s="2">
         <v>5</v>
       </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="48" t="s">
+      <c r="F12" s="59"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="68"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="18"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="25"/>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="57"/>
+      <c r="B13" s="2">
+        <v>9</v>
+      </c>
       <c r="C13" s="11">
         <v>45212</v>
       </c>
@@ -1277,33 +1276,35 @@
       <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="48" t="s">
+      <c r="F13" s="59"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="48"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="68"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="18"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="57"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="11"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="70"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="F14" s="60"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="7">
+        <v>10</v>
+      </c>
       <c r="C15" s="13">
         <v>45207</v>
       </c>
@@ -1313,24 +1314,26 @@
       <c r="E15" s="7">
         <v>3</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="77">
         <v>4</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="58" t="s">
+      <c r="H15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="86" t="s">
+      <c r="I15" s="55"/>
+      <c r="J15" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="87"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="20"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="53"/>
+      <c r="B16" s="7">
+        <v>11</v>
+      </c>
       <c r="C16" s="13">
         <v>45208</v>
       </c>
@@ -1340,18 +1343,20 @@
       <c r="E16" s="7">
         <v>3</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="60" t="s">
+      <c r="F16" s="78"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="89"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="20"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="46"/>
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+      <c r="B17" s="7">
+        <v>12</v>
+      </c>
       <c r="C17" s="13">
         <v>45207</v>
       </c>
@@ -1361,33 +1366,37 @@
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="57" t="s">
+      <c r="F17" s="78"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="57"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="89"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="20"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="53"/>
+      <c r="B18" s="7">
+        <v>13</v>
+      </c>
       <c r="C18" s="13"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="91"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="F18" s="79"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="48"/>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="5">
+        <v>14</v>
+      </c>
       <c r="C19" s="14">
         <v>45208</v>
       </c>
@@ -1397,24 +1406,26 @@
       <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="66">
         <v>5</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="61"/>
-      <c r="J19" s="71" t="s">
+      <c r="I19" s="52"/>
+      <c r="J19" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="72"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
-      <c r="B20" s="21"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="5">
+        <v>15</v>
+      </c>
       <c r="C20" s="14">
         <v>45210</v>
       </c>
@@ -1424,18 +1435,20 @@
       <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="61" t="s">
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="61"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="74"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
-      <c r="B21" s="21"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="52"/>
+      <c r="B21" s="5">
+        <v>16</v>
+      </c>
       <c r="C21" s="14">
         <v>45208</v>
       </c>
@@ -1445,99 +1458,101 @@
       <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="61" t="s">
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="61"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="74"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
-      <c r="B22" s="21"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="52"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="14"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="74"/>
-    </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62" t="s">
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="15"/>
       <c r="D23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="62" t="s">
+      <c r="G23" s="69"/>
+      <c r="H23" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="62"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="74"/>
-    </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
-      <c r="B24" s="22"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="51"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="15"/>
       <c r="D24" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="62" t="s">
+      <c r="G24" s="70"/>
+      <c r="H24" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="62"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="74"/>
-    </row>
-    <row r="25" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="22"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="51"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="15"/>
       <c r="D25" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="62" t="s">
+      <c r="G25" s="70"/>
+      <c r="H25" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="62"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="74"/>
-    </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="22"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="74"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
+      <c r="G26" s="71"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="5">
+        <v>17</v>
+      </c>
       <c r="C27" s="14">
         <v>45221</v>
       </c>
@@ -1547,22 +1562,24 @@
       <c r="E27" s="5">
         <v>3</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F27" s="66">
         <v>8</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="61" t="s">
+      <c r="H27" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="61"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="74"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
-      <c r="B28" s="21"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="52"/>
+      <c r="B28" s="5">
+        <v>18</v>
+      </c>
       <c r="C28" s="14">
         <v>45224</v>
       </c>
@@ -1572,18 +1589,20 @@
       <c r="E28" s="5">
         <v>3</v>
       </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="61" t="s">
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="61"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="74"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
-      <c r="B29" s="21"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="52"/>
+      <c r="B29" s="5">
+        <v>19</v>
+      </c>
       <c r="C29" s="14">
         <v>45221</v>
       </c>
@@ -1593,99 +1612,101 @@
       <c r="E29" s="5">
         <v>2</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="61" t="s">
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="61"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="74"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
-      <c r="B30" s="21"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="52"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="14"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="74"/>
-    </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62" t="s">
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="22"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="15"/>
       <c r="D31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="62" t="s">
+      <c r="G31" s="69"/>
+      <c r="H31" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="62"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="74"/>
-    </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="22"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="51"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="15"/>
       <c r="D32" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="62" t="s">
+      <c r="G32" s="70"/>
+      <c r="H32" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="62"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="74"/>
-    </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="22"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="51"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="15"/>
       <c r="D33" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="62" t="s">
+      <c r="G33" s="70"/>
+      <c r="H33" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="62"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="74"/>
-    </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
-      <c r="B34" s="22"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="51"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
+      <c r="G34" s="71"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="33"/>
+    </row>
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="23"/>
+      <c r="B35" s="4">
+        <v>20</v>
+      </c>
       <c r="C35" s="16">
         <v>45219</v>
       </c>
@@ -1695,24 +1716,26 @@
       <c r="E35" s="4">
         <v>2</v>
       </c>
-      <c r="F35" s="42">
+      <c r="F35" s="74">
         <v>7</v>
       </c>
-      <c r="G35" s="42" t="s">
+      <c r="G35" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="64" t="s">
+      <c r="H35" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="64"/>
-      <c r="J35" s="77" t="s">
+      <c r="I35" s="49"/>
+      <c r="J35" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="K35" s="78"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
-      <c r="B36" s="23"/>
+      <c r="K35" s="35"/>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="49"/>
+      <c r="B36" s="4">
+        <v>21</v>
+      </c>
       <c r="C36" s="16">
         <v>45221</v>
       </c>
@@ -1722,18 +1745,20 @@
       <c r="E36" s="4">
         <v>2</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="64" t="s">
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="I36" s="64"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="80"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
-      <c r="B37" s="23"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="49"/>
+      <c r="B37" s="4">
+        <v>22</v>
+      </c>
       <c r="C37" s="16">
         <v>45219</v>
       </c>
@@ -1743,33 +1768,33 @@
       <c r="E37" s="4">
         <v>1</v>
       </c>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="64" t="s">
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="64"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="80"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="64"/>
-      <c r="B38" s="23"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="37"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="49"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="16"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="80"/>
-    </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="63" t="s">
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="37"/>
+    </row>
+    <row r="39" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="24"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="17"/>
       <c r="D39" s="10" t="s">
         <v>18</v>
@@ -1777,16 +1802,16 @@
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="63" t="s">
+      <c r="H39" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="63"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="80"/>
-    </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="63"/>
-      <c r="B40" s="24"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="37"/>
+    </row>
+    <row r="40" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="50"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="17"/>
       <c r="D40" s="10" t="s">
         <v>19</v>
@@ -1794,16 +1819,16 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="63" t="s">
+      <c r="H40" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="63"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="80"/>
-    </row>
-    <row r="41" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="63"/>
-      <c r="B41" s="24"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="37"/>
+    </row>
+    <row r="41" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="50"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="17"/>
       <c r="D41" s="10" t="s">
         <v>20</v>
@@ -1811,31 +1836,31 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="H41" s="63" t="s">
+      <c r="H41" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="63"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="80"/>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="63"/>
-      <c r="B42" s="24"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="37"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="50"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="17"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="79"/>
-      <c r="K42" s="80"/>
-    </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="64" t="s">
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="37"/>
+    </row>
+    <row r="43" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="23"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="16"/>
       <c r="D43" s="4" t="s">
         <v>18</v>
@@ -1843,16 +1868,16 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="64" t="s">
+      <c r="H43" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="64"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="80"/>
-    </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="64"/>
-      <c r="B44" s="23"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="37"/>
+    </row>
+    <row r="44" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="49"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="16"/>
       <c r="D44" s="4" t="s">
         <v>19</v>
@@ -1860,16 +1885,16 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="64" t="s">
+      <c r="H44" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="64"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="80"/>
-    </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="64"/>
-      <c r="B45" s="23"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="37"/>
+    </row>
+    <row r="45" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="49"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="16"/>
       <c r="D45" s="4" t="s">
         <v>20</v>
@@ -1877,25 +1902,25 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="64" t="s">
+      <c r="H45" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I45" s="64"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="80"/>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="64"/>
-      <c r="B46" s="23"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="37"/>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="49"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="16"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="81"/>
-      <c r="K46" s="82"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="39"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:K46" xr:uid="{784DA642-760B-4062-9544-643C79FF24CC}">
@@ -1903,6 +1928,66 @@
     <filterColumn colId="9" showButton="0"/>
   </autoFilter>
   <mergeCells count="76">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="F35:F38"/>
     <mergeCell ref="J3:K14"/>
     <mergeCell ref="J19:K34"/>
     <mergeCell ref="J35:K46"/>
@@ -1919,66 +2004,6 @@
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="G23:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
The admin functionality works: adding, removing, and creating all work and connect to db
</commit_message>
<xml_diff>
--- a/Documentation/Planning.xlsx
+++ b/Documentation/Planning.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF7E693-23A3-5B4A-BEB3-45C1B8A186CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04194E1-A462-4DA1-BB6F-C99C047B3EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,123 +475,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -605,24 +491,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
@@ -631,24 +499,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -658,9 +508,39 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -669,6 +549,126 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -961,41 +961,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.46484375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.46484375" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="9.1328125" style="1"/>
     <col min="10" max="10" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
+    <col min="11" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-    </row>
-    <row r="2" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+    </row>
+    <row r="2" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1017,17 +1017,17 @@
       <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42" t="s">
+      <c r="I2" s="80"/>
+      <c r="J2" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="42"/>
-    </row>
-    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="K2" s="80"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
@@ -1048,17 +1048,17 @@
       <c r="G3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="22" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="23"/>
-    </row>
-    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="57"/>
+      <c r="K3" s="61"/>
+    </row>
+    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="22"/>
       <c r="B4" s="2">
         <v>4</v>
       </c>
@@ -1077,15 +1077,15 @@
       <c r="G4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="22"/>
       <c r="B5" s="2">
         <v>5</v>
       </c>
@@ -1101,18 +1101,18 @@
       <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="61" t="s">
+      <c r="H5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="63"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="22"/>
       <c r="B6" s="2">
         <v>6</v>
       </c>
@@ -1128,16 +1128,16 @@
       <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="61" t="s">
+      <c r="G6" s="29"/>
+      <c r="H6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="63"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3"/>
@@ -1149,18 +1149,18 @@
         <v>2</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="80" t="s">
+      <c r="G7" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="63"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="24"/>
       <c r="B8" s="3"/>
       <c r="C8" s="12"/>
       <c r="D8" s="3" t="s">
@@ -1170,16 +1170,16 @@
         <v>1</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="63" t="s">
+      <c r="G8" s="31"/>
+      <c r="H8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="63"/>
+    </row>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="24"/>
       <c r="B9" s="3"/>
       <c r="C9" s="12"/>
       <c r="D9" s="3" t="s">
@@ -1189,29 +1189,29 @@
         <v>1</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="65" t="s">
+      <c r="G9" s="31"/>
+      <c r="H9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="62"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="63"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="24"/>
       <c r="B10" s="3"/>
       <c r="C10" s="12"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+      <c r="G10" s="32"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="63"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2">
@@ -1226,21 +1226,21 @@
       <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="33">
         <v>6</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="G11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="57" t="s">
+      <c r="H11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
-    </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="63"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="22"/>
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -1253,17 +1253,17 @@
       <c r="E12" s="2">
         <v>5</v>
       </c>
-      <c r="F12" s="59"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="57" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="22"/>
       <c r="B13" s="2">
         <v>9</v>
       </c>
@@ -1276,30 +1276,30 @@
       <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="57" t="s">
+      <c r="F13" s="34"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="57"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="63"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="22"/>
       <c r="B14" s="2"/>
       <c r="C14" s="11"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="65"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="7">
@@ -1314,23 +1314,23 @@
       <c r="E15" s="7">
         <v>3</v>
       </c>
-      <c r="F15" s="77">
+      <c r="F15" s="41">
         <v>4</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="54" t="s">
+      <c r="H15" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="55"/>
-      <c r="J15" s="43" t="s">
+      <c r="I15" s="39"/>
+      <c r="J15" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="44"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
+      <c r="K15" s="82"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="37"/>
       <c r="B16" s="7">
         <v>11</v>
       </c>
@@ -1343,17 +1343,17 @@
       <c r="E16" s="7">
         <v>3</v>
       </c>
-      <c r="F16" s="78"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="56" t="s">
+      <c r="F16" s="42"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="53"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="46"/>
-    </row>
-    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="37"/>
       <c r="B17" s="7">
         <v>12</v>
       </c>
@@ -1366,32 +1366,32 @@
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="78"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="53" t="s">
+      <c r="F17" s="42"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="46"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="53"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="84"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="37"/>
       <c r="B18" s="7">
         <v>13</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="48"/>
-    </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="s">
+      <c r="F18" s="43"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="86"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="47" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="5">
@@ -1406,23 +1406,23 @@
       <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="48">
         <v>5</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="52"/>
-      <c r="J19" s="28" t="s">
+      <c r="I19" s="47"/>
+      <c r="J19" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
+      <c r="K19" s="67"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="47"/>
       <c r="B20" s="5">
         <v>15</v>
       </c>
@@ -1435,17 +1435,17 @@
       <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="52" t="s">
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="52"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="31"/>
-    </row>
-    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="69"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="47"/>
       <c r="B21" s="5">
         <v>16</v>
       </c>
@@ -1458,29 +1458,29 @@
       <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="52" t="s">
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="52"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="31"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="69"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="47"/>
       <c r="B22" s="5"/>
       <c r="C22" s="14"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="31"/>
-    </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="69"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" s="51" t="s">
         <v>10</v>
       </c>
@@ -1491,15 +1491,15 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="69"/>
+      <c r="G23" s="52"/>
       <c r="H23" s="51" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="51"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="31"/>
-    </row>
-    <row r="24" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" s="51"/>
       <c r="B24" s="6"/>
       <c r="C24" s="15"/>
@@ -1508,15 +1508,15 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="70"/>
+      <c r="G24" s="53"/>
       <c r="H24" s="51" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="51"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="31"/>
-    </row>
-    <row r="25" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" s="51"/>
       <c r="B25" s="6"/>
       <c r="C25" s="15"/>
@@ -1525,29 +1525,29 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="70"/>
+      <c r="G25" s="53"/>
       <c r="H25" s="51" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="51"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" s="51"/>
       <c r="B26" s="6"/>
       <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="71"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="31"/>
-    </row>
-    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="52" t="s">
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="47" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="5">
@@ -1562,21 +1562,21 @@
       <c r="E27" s="5">
         <v>3</v>
       </c>
-      <c r="F27" s="66">
+      <c r="F27" s="48">
         <v>8</v>
       </c>
-      <c r="G27" s="66" t="s">
+      <c r="G27" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="52"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="31"/>
-    </row>
-    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="47"/>
       <c r="B28" s="5">
         <v>18</v>
       </c>
@@ -1589,17 +1589,17 @@
       <c r="E28" s="5">
         <v>3</v>
       </c>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="52" t="s">
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="52"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="31"/>
-    </row>
-    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="52"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="47"/>
       <c r="B29" s="5">
         <v>19</v>
       </c>
@@ -1612,29 +1612,29 @@
       <c r="E29" s="5">
         <v>2</v>
       </c>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="52" t="s">
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="52"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="31"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="52"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="47"/>
       <c r="B30" s="5"/>
       <c r="C30" s="14"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="31"/>
-    </row>
-    <row r="31" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="69"/>
+    </row>
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="51" t="s">
         <v>12</v>
       </c>
@@ -1645,15 +1645,15 @@
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="69"/>
+      <c r="G31" s="52"/>
       <c r="H31" s="51" t="s">
         <v>23</v>
       </c>
       <c r="I31" s="51"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="31"/>
-    </row>
-    <row r="32" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="68"/>
+      <c r="K31" s="69"/>
+    </row>
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="51"/>
       <c r="B32" s="6"/>
       <c r="C32" s="15"/>
@@ -1662,15 +1662,15 @@
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="70"/>
+      <c r="G32" s="53"/>
       <c r="H32" s="51" t="s">
         <v>25</v>
       </c>
       <c r="I32" s="51"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="31"/>
-    </row>
-    <row r="33" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="68"/>
+      <c r="K32" s="69"/>
+    </row>
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="51"/>
       <c r="B33" s="6"/>
       <c r="C33" s="15"/>
@@ -1679,29 +1679,29 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="70"/>
+      <c r="G33" s="53"/>
       <c r="H33" s="51" t="s">
         <v>24</v>
       </c>
       <c r="I33" s="51"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="31"/>
-    </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="68"/>
+      <c r="K33" s="69"/>
+    </row>
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" s="51"/>
       <c r="B34" s="6"/>
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="71"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="51"/>
       <c r="I34" s="51"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="33"/>
-    </row>
-    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="49" t="s">
+      <c r="J34" s="70"/>
+      <c r="K34" s="71"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="56" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="4">
@@ -1716,23 +1716,23 @@
       <c r="E35" s="4">
         <v>2</v>
       </c>
-      <c r="F35" s="74">
+      <c r="F35" s="57">
         <v>7</v>
       </c>
-      <c r="G35" s="74" t="s">
+      <c r="G35" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="49" t="s">
+      <c r="H35" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="49"/>
-      <c r="J35" s="34" t="s">
+      <c r="I35" s="56"/>
+      <c r="J35" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="K35" s="35"/>
-    </row>
-    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="49"/>
+      <c r="K35" s="73"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="56"/>
       <c r="B36" s="4">
         <v>21</v>
       </c>
@@ -1745,17 +1745,17 @@
       <c r="E36" s="4">
         <v>2</v>
       </c>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="49" t="s">
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="I36" s="49"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="37"/>
-    </row>
-    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="75"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="56"/>
       <c r="B37" s="4">
         <v>22</v>
       </c>
@@ -1768,30 +1768,30 @@
       <c r="E37" s="4">
         <v>1</v>
       </c>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="49" t="s">
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="49"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="37"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="75"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="56"/>
       <c r="B38" s="18"/>
       <c r="C38" s="16"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="37"/>
-    </row>
-    <row r="39" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50" t="s">
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="75"/>
+    </row>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="55" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="19"/>
@@ -1802,15 +1802,15 @@
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="50" t="s">
+      <c r="H39" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="50"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="37"/>
-    </row>
-    <row r="40" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="75"/>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="55"/>
       <c r="B40" s="19"/>
       <c r="C40" s="17"/>
       <c r="D40" s="10" t="s">
@@ -1819,15 +1819,15 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="50" t="s">
+      <c r="H40" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="50"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="37"/>
-    </row>
-    <row r="41" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="50"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="75"/>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="55"/>
       <c r="B41" s="19"/>
       <c r="C41" s="17"/>
       <c r="D41" s="10" t="s">
@@ -1836,28 +1836,28 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="H41" s="50" t="s">
+      <c r="H41" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="50"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="37"/>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="50"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="75"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="55"/>
       <c r="B42" s="19"/>
       <c r="C42" s="17"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="37"/>
-    </row>
-    <row r="43" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="75"/>
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="56" t="s">
         <v>17</v>
       </c>
       <c r="B43" s="18"/>
@@ -1868,15 +1868,15 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="37"/>
-    </row>
-    <row r="44" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="49"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="75"/>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="56"/>
       <c r="B44" s="18"/>
       <c r="C44" s="16"/>
       <c r="D44" s="4" t="s">
@@ -1885,15 +1885,15 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="49" t="s">
+      <c r="H44" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="49"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="37"/>
-    </row>
-    <row r="45" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="49"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="75"/>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="56"/>
       <c r="B45" s="18"/>
       <c r="C45" s="16"/>
       <c r="D45" s="4" t="s">
@@ -1902,25 +1902,25 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="49" t="s">
+      <c r="H45" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="I45" s="49"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="37"/>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="49"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="75"/>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="56"/>
       <c r="B46" s="18"/>
       <c r="C46" s="16"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="49"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="39"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="77"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:K46" xr:uid="{784DA642-760B-4062-9544-643C79FF24CC}">
@@ -1928,66 +1928,6 @@
     <filterColumn colId="9" showButton="0"/>
   </autoFilter>
   <mergeCells count="76">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="F35:F38"/>
     <mergeCell ref="J3:K14"/>
     <mergeCell ref="J19:K34"/>
     <mergeCell ref="J35:K46"/>
@@ -2004,6 +1944,66 @@
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>